<commit_message>
Get daily reddit data: Tue Dec  5 08:08:43 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_12_10.xlsx
+++ b/data/2023_12_10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C442"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,2403 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>18b73d9</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Nail Gift Idea for Girlfriend</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18b73d9/nail_gift_idea_for_girlfriend/</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>18b6w0j</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>From Halloween</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/971jkccukf4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>18b6vyq</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Lumpy overlay</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18b6vyq</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>18b6vy8</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Winter nails on client!</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r2rm3nkskf4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>18b6mu8</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Dupe for OPI my favorite ornament?</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18b6mu8/dupe_for_opi_my_favorite_ornament/</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>18b6gya</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Late fall mani</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18b6gya</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>18b5ick</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Beetles gel polish question :)</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18b5ick/beetles_gel_polish_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>18b46dp</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Christmas nails, 1st set</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18b46dp</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>18b2pn0</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>The Nails and the Inspiration</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18b2pn0</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>18b2dhj</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Reposting because I forgot to tag. First time trying blue nails! Second pic is inspo from purenailsbyemma, found in Google!</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18b2dhj</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>18b3x4a</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Festive nails</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18b3x4a</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>18b3vdj</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>looking for picture to show nail artist</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18b3vdj/looking_for_picture_to_show_nail_artist/</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>18b3qex</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Pinkie natural nail completely cracked horizontal - suggestions to protect it while it grows out?</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/em8n9btyle4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>18b3l71</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Working on gem placement</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18b3l71</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>18b3dv8</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>French tip nails by myself</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18b3dv8</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>18b1huh</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Gingerbread nails 🎄</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s5o189h71e4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>18b13gt</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Nail color</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18b13gt</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>18azweb</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>I’m a dude and these are my new nails I did on myself</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18azweb</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>18aye5t</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>First time trying Kiss Salon Xtend.</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ncq0xg6kad4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>18axyy3</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>My first time doing my own nail art</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18axyy3</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>18awgnr</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Does this look natural?</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18awgnr</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>18axqeb</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Nails I’ve done recently that I’m super proud of!</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1xed8g985d4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>18axous</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Painted my nails for the first time in my life. Never again🥲.</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8rop7uww4d4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>18axlvn</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Christmas nails🤍❤️</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8v7e8ky94d4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>18axg0j</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>In love with the OPI Dutch Tulips shade 🩷</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m9bg0xy03d4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>18ax5zc</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>My beautiful nails 🔥😍😍</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s984mbow0d4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>18awxnf</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Chrome gold claws</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t2gm3u35zc4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>18awaei</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>A little winter sparkle for the holidays (press on)</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rt2y61s4uc4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>18avy9k</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>My friend's work. Choose your fav design</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18avy9k</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>18avwt1</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Different salon redoing my polish?</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18avwt1/different_salon_redoing_my_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>18arnzx</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Just got Xmas lights!</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kav3qxdwub4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>18armgl</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Broken nails very often</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c4g4yk4lub4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>18aqaih</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>How do I strengthen my nails?</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18aqaih</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>18ap9xe</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>why do my acrylic nails always lift up at the cuticle?</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18ap9xe/why_do_my_acrylic_nails_always_lift_up_at_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>18avqt5</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Which nail shape suits me better?</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18avqt5</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>18avkh3</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Rudolph the..silver nosed reindeer had a very shiny nose 😂</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ebiyrbmoc4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>18avfdx</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Winter nails flop</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k3rd3cainc4c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>18alchx</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>How to get glue off of pre-glued press on nails?</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18alchx/how_to_get_glue_off_of_preglued_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>18akd2r</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Christmas 🎄 ideas?</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18akd2r/christmas_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>18ak2ks</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Shape advice for DIY nails</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ak2ks</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>18av8tt</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Green for the festival holiday.</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y3vhzhy3mc4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>18av6lr</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Feeling Festive! 🎄</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s71locholc4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>18av0ye</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Pink and gold nails</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hf1b44tfkc4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>18av02h</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Please help me</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18av02h</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>18aimqf</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Recommendations for Christmas present?</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18aimqf/recommendations_for_christmas_present/</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>18auqr5</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Help with my builder gel skills?</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18auqr5</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>18aulnh</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Press ones that looked like acrylics</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7hs26005hc4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>18au035</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>🍪 ILNP Cookie Cutter, Toasted, and Birthday Suit 🌟</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18au035</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>18atele</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>I tried 3D nail art for the 1st time! (Ignore the peeling on my thumb— boiling water accident)</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18atele</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>18asx4d</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>I’ll die for this color combo🖤</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cdjrogpa4c4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>18aslkn</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Why do my dip nails look like this?</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xucvhftw1c4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>18as2qo</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Pink 💖</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b8svf3v0yb4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>18as1zn</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>First time with nails this long</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kau8uy2vxb4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>18arwfc</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Sparkly winter nails for myself!</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18arwfc</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>18arh68</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Press on nails I spiced up !</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18arh68</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>18are73</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Newbie to nails and want extensions</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18are73/newbie_to_nails_and_want_extensions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>18ara70</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Need opinions</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ara70</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>18ar9dp</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Looking for an opal polish (gel)</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ar9dp</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>18aqmqm</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>olive my olive nails</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5gjj10m2nb4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>18aq3uu</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>my melody christmas nails ⋆˙⟡♡</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18aq3uu</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>18aq3ca</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>green and gold combo &gt;</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18aq3ca</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>18aplsb</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Happy holidays!</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dd5zucm6fb4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>18apaq4</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Braille Nail Art (Christmas)</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18apaq4</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>18ap4ks</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Birthday nails</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ha548kbhbb4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>18aoxvf</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>It appears I may have inadvertently channeled Nacho Libre at my last nail appointment 😬</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18aoxvf</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>18aoi5o</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Pre Christmas nails</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/de4bzgbi6b4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>18aocb9</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>What are the differences for nail options ?</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18aocb9/what_are_the_differences_for_nail_options/</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>18ao787</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>First set of Poly Gel nails</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f5iwf0a64b4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>18anwd6</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Press on nails float because they're not curved enough</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18anwd6</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>18anvi3</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>My very first attempt at anything else but a solid color 😅</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jiitkm2k1b4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>18anr1j</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>little aura nails &lt;3</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/46makali0b4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>18and1n</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Had a panic attack and peeled the polish off my already brittle nails, any advice on what I can do to help them grow out better?</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tb2i4m6bxa4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>18amywh</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>I broke my pointer finger nail. Does this look stupid if I just wait till it grows out? Or should I clip the rest 🫠</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18amywh</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>18amvwv</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Hello, Christmas!</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1flqpelhta4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>18amvvr</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>smells like candied peppermint. 🥰🎄🍭✨</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18amvvr</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>18amdni</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Some winter Wu, and a Christmas tree, too❄️</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18amdni</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>18akwqp</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Best opaque white polish/lacquer? 🤔</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18akwqp/best_opaque_white_polishlacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>18aiwjy</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>First time making press ons</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jqpgkphnr94c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>18aikbw</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>advice please!!</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18aikbw/advice_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>18ahxk1</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Cute little bears!</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/io6r3vtvf94c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>18ahcgm</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Red the classic</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vuzkhayd894c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>18agewo</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>gingerbread man nails</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/28p0d6liv84c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>18afxmg</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>switched my stilettos for coffins!</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18afxmg</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>18b4gis</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Finally got zoya sale order - Rocky</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nvamgqp5te4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>18b3qmr</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>A simple, sparkly holiday dotticure ✨</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6snljsx0me4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>18b3pxk</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>New Mani for the Week</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18b3pxk</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>18b2ptv</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Finnish polish Lumene</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zmrwp9cace4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>18b048x</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>First taste of Sassy Sauce</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18b048x</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>18aztzu</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>ILNP Revival ✨️</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18aztzu</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>18azqxy</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>a yule frosting</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18azqxy</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>18azlf2</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Photos don't do it justice - Kiss Me by Cadillacquer</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18azlf2</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>18az66j</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Builder in a bottle lifting on the edges?</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18az66j</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>18ayija</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Mooncat VR 🌹</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ptrtimibd4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>18aygik</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>lookin fly for a cacti 🌵</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18aygik</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>18aygi6</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Blue and Silver Snowflake Mani</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dlnhtyx2bd4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>18ay5ob</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Day 4 of 12 days of Nails</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w5z3c9ho8d4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>18av4vl</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Essie - Swoon in the Lagoon</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18av4vl</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>18axasm</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Orly - Cake Pop + Poparazzi - Star Shine</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18axasm</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>18awti0</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Ethereal Lacquer’s Hunt 🌬️</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kqamhkk8yc4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>18awtba</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>My First Bees Knees purchase 😍✨🍋🐝</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/q9jpbq96yc4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>18awdmp</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Friends with nickel allergies/sensitivities - does magnetic polish with nickel (ie Mooncat Velvet Rose) give you a reaction?</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18awdmp/friends_with_nickel_allergiessensitivities_does/</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>18avcci</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Are these Christmasy enough?</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6gdw03avmc4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>18aulba</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>So velvety</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sz6is1j1hc4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>18au7dy</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>cirque colours - canada</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18au7dy/cirque_colours_canada/</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>18au6b8</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Braille Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18au6b8</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>18atw9j</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>🍪 ILNP Cookie Cutter, Toasted, and Birthday Suit 🌟</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18atw9j</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>18atjj2</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Nail filing help!</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18atjj2/nail_filing_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>18apesk</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Dazzle Dry over Dip Manicure?</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18apesk/dazzle_dry_over_dip_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>18atcw0</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Cozy Sweater Nails</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mg84n4vl7c4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>18asjuh</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Definitely a new favorite!</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18asjuh</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>18asemf</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Any suggestions for a “dusty” pink for a subtle *my nails but better* palate cleanser? Disappointed in Essie sugar daddy</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18asemf</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>18aqag6</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Twisted Terracotta Tanzanite!</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18aqag6</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>18apogk</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>A love for sheers and jellies</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4wia4szsfb4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>18ap1y0</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Blue and Gold</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zfcrbf7vab4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>18aoecq</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>ILNP Sugar Plum💜</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/b4gtea0l5b4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>18anj9i</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Christmas nail art</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fmk37iopya4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>18anb5j</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Holo Taco "Curfew Crasher"</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kxb9zukvwa4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>18an8ue</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Holo Taco "Cool Cat Mom</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9usbhcbfwa4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>18amudy</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>smells like candied peppermint. 🥰🎄🍭✨</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18amudy</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>18ampd3</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Ghost Rose on this rainy Monday</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1oheu9hyra4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>18ammb6</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Nail Polish cleaner</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18ammb6/nail_polish_cleaner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>18amlfh</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>ILNP Deep Space - First attempt at velvet effect, pleasantly surprised!</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0h5mv6j1ra4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>18am3aw</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>'tis the season for not-quite-black shades</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tk2pn0wlma4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>18al336</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Christmas Pairing - Mooncat "My Bugs, My Bugs" and Sassy Sauce "Chicago Fire"</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18al336</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>18ak60n</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>my first time with gel polish. Some advice?</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ak60n</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>18ak2mp</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>I’ll give you three guesses as to how I broke my thumb nail and exactly what I was planning to do right after making breakfast.</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b2ypvwh54a4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>18ajy4c</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Perfect lighting</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pzpvoi7u2a4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>18ajhcm</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Chrome nails with white gel polish</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ajhcm</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>18ahve3</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18ahve3/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>18ahefn</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>abstract christmas ❄️ love doing these! (__kmnails)</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uc0aqyz6994c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>18ag42d</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Nail Stamping Attempt #1</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ag42d</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>18ag1xk</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Sunshine and Sugar Plum</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j9pzt2geq84c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>18b0i1v</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Stamping time</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/timi0lwgsd4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>18azc9m</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Had the time of my life with these!</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18azc9m</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>18az2lg</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Some of my first attempts at gel extensions</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18az2lg</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>18awyyh</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Tried a new one today</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t1rad9ifzc4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>18asbds</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Braille Nail Art (Christmas)</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18asbds</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>18ar8st</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>DIY cat eye gel nails I’m so proud of it 💖💖</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n6x8lxiqrb4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>18apwdu</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>I'm in love with these press ons! 💜</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/duc3wfvhhb4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>18am9f8</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>My client asked me for something Christmas, I'm new to this, please leave your opinion</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w3fp2yk4oa4c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>18alw6u</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>I made Bluey nails</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18alw6u</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Dec  6 08:08:24 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_12_10.xlsx
+++ b/data/2023_12_10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C442"/>
+  <dimension ref="A1:C603"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7947,6 +7947,2743 @@
         </is>
       </c>
     </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>18byz2a</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Favourite manicures</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18byz2a</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>18by8v3</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Almond nails</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h2n0kz7ygm4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>18bxsk4</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Where to buy polish in Canada</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18bxsk4/where_to_buy_polish_in_canada/</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>18bwd67</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Are my natural nails too long?</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v9lchfy9wl4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>18bw5xt</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Im very proud of these and wanted to share them 🥹</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bw5xt</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>18bvw2u</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>I’m having trouble getting onboard with holiday nails bc I’m really into cats</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/khpfbcpkrl4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>18bv21i</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Improper Gel X application? I don’t think this was worth $145. I’m unhappy. Thoughts?</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l7thljyijl4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>18buyi4</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>What is this and how can I get rid of them?</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18buyi4</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>18butqh</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>In love with my nails 😍😍😍</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5xxe6g4chl4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>18buttd</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Couldn’t pick just one so I did both 😍</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18buttd</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>18buqkn</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Second time ever doing gel x nails</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yemwchgjgl4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>18bu61q</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Do glitter gels last longer than regular gel?</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ib5b6yabl4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>18btowg</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>No nails, yet! What should I do?</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l7f7h0v37l4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>18btie7</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>I really miss having an excuse to put pumpkins on my nails</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wophuwgf5l4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>18btanc</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>So excited to be able to start Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18btanc</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>18bt664</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Christmas gnome!</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bt664</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>18bt4jz</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>My first time doing nail art on someone else. Turned out a lot better than i expected ☺️</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bt4jz</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>18bslml</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Pinkmas</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bslml</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>18bs8rd</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Christmas nail comp</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bs8rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>18bs5g5</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Festive blue and silver</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bs5g5</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>18bruws</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Holiday nails!</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nwy0mhzjqk4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>18brq1a</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Are there any acrylate free nail glues?</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18brq1a/are_there_any_acrylate_free_nail_glues/</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>18brhzl</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Too pink?</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8no1mfphnk4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>18bqxc2</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>The smallest Totoro scenario nail set 💚</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bqxc2</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>18bquvi</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>My Christmas nails, done by my incredible tech 😍</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bquvi</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>18bqqlr</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Thought?</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hfeui5qxgk4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>18bqopd</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>What nail color would you get to compliment this dress?</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18bqopd/what_nail_color_would_you_get_to_compliment_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>18bqc65</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Old Ipsy stickers ☺️</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h1bs81oodk4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>18bq1y1</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Green faded nails matching bracelet</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bq1y1</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>18bprpn</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>My gel manicure always peels off</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18bprpn/my_gel_manicure_always_peels_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>18bpewr</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>A Pink Christmas</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bpewr</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>18bp2d1</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Pink Christmas 🩷❄️</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bp2d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>18bow35</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>minimalist nails (gel)</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hdqbbczq2k4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>18bopps</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>I did these nails on a client last week using sculpted gel products. What do you think!?</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lofr6x3g1k4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>18bo0tf</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Rate my nails 💅 Christmas Sugar cookie with ginger bread themed</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wb4sngcawj4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>18bnuyi</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Winter IS coming</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vyv5zb61vj4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>18bnosw</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Sometimes i love to combine black and tan colours in one manicure</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zd1gf2crtj4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>18bnkpm</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>I started pushing my cuticles as far back as humanly possible before applying gel so that they look less grown out for longer. This is two weeks of wear. I think it helps!</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zm5fra8ysj4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>18bnht6</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Was Feeling Flashy</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/92zcoe8dsj4c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>18bn53k</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Yes / no?🌹</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ytdz5zqpj4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>18bn0ny</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Tips for low quality nail polish</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/99ayqq8uoj4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>18bmsg9</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>My new set for Christmas</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tc6o1i84nj4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>18bmngu</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Gingerbread nails</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bmngu</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>18blilh</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Simple red glitter set❤️</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nkxoqkbndj4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>18blgjc</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>I fell in love with manicures with full cover tips, are they easy to apply? I'm a beginner</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18blgjc/i_fell_in_love_with_manicures_with_full_cover/</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>18bl60l</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>My last set!</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q7jomkv0bj4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>18bl2n7</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>My Barbie nails</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tv41as2baj4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>18bkzpm</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>My friend did my nails today!!! They are so cute on my natural nail🥹❤️</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bkzpm</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>18bksqj</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>My (not super on the nose) christmas nails!</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/swd0l1z98j4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>18bkrsg</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Simple but beautiful Xmas mani</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c782rji38j4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>18bk9ni</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Shoutout to Japan for these</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zirrf09a4j4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>18bju7e</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>How do we feel about this set of nails I did?</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/typ3fra01j4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>18bjozh</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Red nails ft ribbons</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bjozh</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>18bjlrp</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Sparkly nails</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zanwfnnazi4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>18bjb46</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Christmas nails (:</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xztea8jywi4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>18bja1a</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Christmas nail art.</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vr2xvvkpwi4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>18biorq</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Holiday red and silver for the rest of the year!</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18biorq</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>18bihpe</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Winter wonderland press ons! These are gel!</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xhg3f30mqi4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>18bih3u</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Feeling a little festive 💅🏻</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lgs2x0fiqi4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>18bif9z</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Acrylic glitter snowflake press ons! </t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g5z5gkg4qi4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>18bifp9</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Winter wonderland dip</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a8m9oi58qi4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>18bi3q1</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Picked up a new hobby of doing gel nails!</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bi3q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>18bhjmd</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>My nail stamp won’t pick up the print. Any reason why? Thanks.</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fzwgi4efji4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>18bhf9t</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Black Christmas nails.</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0mtt35bhii4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>18bh4px</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Cowboy Christmas</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bh4px</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>18bgyzg</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Christmas nails (i am terrible at taking pictures)</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bgyzg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>18bgpzc</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Green glitter and gold flakes</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bgpzc</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>18bflxf</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>What color to buy ✨️</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bflxf</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>18ba16n</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Experience with Apres Gel (X) nails?</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18ba16n/experience_with_apres_gel_x_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>18b5u9y</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18b5u9y</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>18bf2q9</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>My new nails...before Christmas!</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18bf2q9/my_new_nailsbefore_christmas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>18begvu</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Plain and blue for winter!</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7229od5awh4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>18bec2s</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>First manicure</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6i4swixbvh4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>18bd9x0</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Please rate my nails :( not happy</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lsnesnkulh4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>18bd8cq</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Hanukkah nails ✡️✨💙</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bd8cq</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>18bctqv</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Since autumn is just about over, here’s my Ode to Fall</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bctqv</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>18bcgew</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Candy cane Christmas nails</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/irwbdcgzeh4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>18bcasa</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Gnomie Nails</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bcasa</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>18baggc</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>abstract christmas nails by me!</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ixfhmn1kug4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>18ba0zt</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Wintery vibes ❄️</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ge9mingpg4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>18b9919</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Gel Top Coat over False Press on Nails</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18b9919/gel_top_coat_over_false_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>18b8mo0</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Cutest ones I’ve found</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18b8mo0</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>18b7rn8</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>I wanted nails that matched my vacation spot</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/defz5yfbwf4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>18byi5z</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>A few of my favourites from over the years 💅</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18byi5z</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>18bxui1</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>always 💙 a good dusty blue</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kgzblk73cm4c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>18bxszb</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Zoya Sage and Pacifica Rainbow Gloss. A little trip down memory lane</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bxszb</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>18bvdeb</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Glitter Season is here!</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bvdeb</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>18bvbg5</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>my tech did her big one yet again. inspo pic at the end this set cost me $80</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bvbg5</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>18bur54</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Christmasy mani 🤶</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bur54</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>18bukuu</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>[PR] ORLY has been crushing it with these fall colors 😩</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bukuu</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>18buko3</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Not Sure About This Color On Me | Cirque Colors Rosewater Jelly</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18buko3</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>18buhb6</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Latest cat eye effort</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sl0v2y91el4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>18buhc7</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>🌙 🐈‍⬛ Gates of Hell</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cv4qv473el4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>18bubbo</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>My first polish from PPU looks sooo good!</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pcspuuzkcl4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>18btr39</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>HOW IS SABERTOOTH SO GLOWY</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18btr39</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>18btl5s</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Dupe request for this base color</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18btl5s</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>18btf1x</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Adding my House of Hades swatch to the gallery</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k9ud2vmk4l4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>18btd4h</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>🎅 Community Christmas Giveaway 🤶</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ikyf35k24l4c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>18bst00</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Makes me think of Christmas lights</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bst00</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>18bsbmk</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Christmas mani 🎄</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g0154dupuk4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>18bsar4</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Looking for a WFL dupe</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3lcbw3thuk4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>18brwve</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Black Friday order finally came! ILNP Bear Hug 🧸🐻</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q49isqi2rk4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>18brqsk</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>I call these naked nails ☺️</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c59ebhkmpk4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>18brqnf</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Color club $1 sale</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18brqnf/color_club_1_sale/</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>18br8wk</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Milk 🥛</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mi728mu8lk4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>18bqaor</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>AITA because I want to paint my nails almost everyday?</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r15shsmadk4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>18bq34j</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Help finding Beetles b159 Dusty Rose Dupe</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18bq34j/help_finding_beetles_b159_dusty_rose_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>18bpwy7</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Hint of silver</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/isx5wt9eak4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>18bpjsi</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Is this blue or black???</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ir3jj14k7k4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>18bpjg6</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Ethereal "Ruhndanaan Knew Three Things With Absolute Certainty"</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ghsx8n3h7k4c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>18bp7h8</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Christmas nails in December- how original</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bp7h8</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>18bokue</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Cuticle oil vs top coat</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5e9d7cze0k4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>18bocwm</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>“Trust the Process”</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bocwm</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>18bnwly</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Can you all point me in the direction of any dupes for HT Spirit Fingers?</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18bnwly/can_you_all_point_me_in_the_direction_of_any/</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>18bnug5</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Which polishes do you think are truely unique - with no others like them?</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18bnug5/which_polishes_do_you_think_are_truely_unique/</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>18bnlzx</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>question about press ons and gel</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/17g91bl7tj4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>18bma8g</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>New to Nail Polish</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g8yko6bfjj4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>18bm52z</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>It looks different in every light, heavy on the mint shimmer but definitely some pink shimmer low lights.</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bm52z</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>18bm4ip</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>This sub was right! Sassy Sauce gorgeous!</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bm4ip</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>18bm0ck</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Does anybody know of a glowy blue sheer polish that doesn’t have a yellow base?</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tg4w68gdhj4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>18bldd2</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Someone either enable me or speak sense &amp; reason to me (re: Cirque Colors sale)</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18bldd2/someone_either_enable_me_or_speak_sense_reason_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>18bl9ss</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>[Looking for a similar shade] Would someone share a nail polish thats close to this shade of pink?</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18bl9ss/looking_for_a_similar_shade_would_someone_share_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>18bl4jf</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>HOH on Nail Wraps for Hanukkah</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/atewp4vpaj4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>18bkuol</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Where to buy shimmer?</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18bkuol/where_to_buy_shimmer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>18bk0d7</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Some rainy day vibes</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bk0d7</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>18bjppv</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Have yourself a vampy little Christmas 🎶</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/58epupf50j4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>18bjnfz</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Zoya’s Daul ✨</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y0atxdzmzi4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>18bjjbu</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>i can’t stop starting at the shiftiness of this polish 🤩</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yem2kasqyi4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>18bjfxn</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>I’d love to see y’all’s nails ‘n’ tails (pets without tails also welcome)</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bjfxn</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>18bivh7</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Thermal nail polish adventures ⛄</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bivh7</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>18bie82</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Fellow laqueristas I have a question</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9dvgqgfxpi4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>18bie4h</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>If I had a dollar....</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xl914nowpi4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>18bibpn</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Ethereal Starsword</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ofbe2urapi4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>18bi5ok</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Tortoise Shell 🐢 obsessed with how it came out and much easier to do than I thought it would be!</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bi5ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>18bfoty</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Question</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18bfoty/question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>18bh6ul</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Perfect lighting in a weird space</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ltijw49ogi4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>18bh4w0</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Help finding a color similar to Essie sand tropez</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18bh4w0/help_finding_a_color_similar_to_essie_sand_tropez/</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>18bh0rd</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Black + Topper</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/nWoa9dX</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>18bgvri</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Am I seeing things or are they different?</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bgvri</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>18bgtib</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Favorite brand of acetone additive?</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18bgtib/favorite_brand_of_acetone_additive/</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>18bgb4y</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>✨️🧩Metallic Puzzle🧩✨️</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bgb4y</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>18bd6mo</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>A Darker Christmas Mani</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2uucc6o3lh4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>18bcuq8</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>A touch of Zen</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bcuq8</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>18bc4jt</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>(PR) Hanukkah nail inspo ✡️💙</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bc4jt</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>18bbppt</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Wine tip sparkly French manicure!</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bbppt</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>18bb9f2</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>First time trying to create a gradient using the sponge technique</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/910zu92c3h4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>18bax31</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>ILNP Candlelight 🖤✨ + ILNP Rosewater 🤍✨</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bax31</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>18bahbo</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>christmas bauble nails handpainted by me! (__kmnails)</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/seqfw5irug4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>18b9eyi</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>A Engand Dracula &amp; The Wizard</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mhkjqdv9ig4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>18bwast</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>New "face" for Dec.</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i2xjmms7vl4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>18bvxnc</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>A couple days ago I posted that I’m not into holiday nails bc i’m really into cats… This is part 2 except this cat is in a sweater so that counts as holiday right??? RIGHT??</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kvizu030sl4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>18bvika</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Oops all holo</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3lf4mfkwnl4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>18bvenu</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Subtle holiday nails using cat eye polish!</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0std2kauml4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>18bs6vx</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>cheetah nails!</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/74dd0czitk4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>18bju8h</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Some of the Christmas nails I did this year 🎄 🎁</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bju8h</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>18bjrlm</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Matching Christmas Nails with my Mom (done by me)</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jg6ghfdj0j4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>18bjqd5</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Did some winter nails but I wish the black would have shown up more. I’m now dreading having to do this with my non-dominant hand. Wish me luck 🥲</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nda7teh90j4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>18bihpn</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>DIY jelly green almond set</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9h79jlxmqi4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>18bexfa</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>I’m incredibly proud of these. I’ve worked so hard trying to learn how to do my own nails, let alone nail art. Not complicated, nothing fancy, but I love these.</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pojv1uphzh4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>18bamr2</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Christmas nails but not red or green, what do you think?</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bamr2</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>18b89qr</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>First festive set ✨ Not my best work, tried a new builder &amp; I HATE it. It made my white gel bleed after fully cured and is so thick makes my nails look chunky ☹️</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18b89qr</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Dec  7 08:08:16 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_12_10.xlsx
+++ b/data/2023_12_10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C603"/>
+  <dimension ref="A1:C772"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10684,6 +10684,2879 @@
         </is>
       </c>
     </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>18cptz3</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Holiday Nails 🥰</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v1g7xswllt4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>18coq9d</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Great tutorials for beginners with short nails?</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18coq9d</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>18cop65</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>White sugar frenchies w/ cute lil xmas lights ☺️ @ xoyanie</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ay0gvtht8t4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>18coerr</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/go3jexsp5t4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>18co4pc</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Chrome nails fail?</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18co4pc</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>18co0az</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>princess nails</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c1cy8qbl1t4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>18cnrx9</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>I made this design</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f8g677ldzs4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>18cnpab</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Negative Space</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cnpab</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>18cnjht</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>I decided to try acrylics, how did I do?</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/41iqtdg0xs4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>18cnjap</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Holiday nails ✨</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x0fe2hpyws4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>18cnc1g</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Got my nails done in Japan!</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cnc1g</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>18cnb0o</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>The Pink Christmas Nails of My Dreams ❄️</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z3p1oocpus4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>18cn0hx</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>tis’ the season ❄️</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cn0hx</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>18cjixq</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Naughty Nails 🙈😂</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kkstfu6qvr4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>18cifbx</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>How do you deal with subborn nails that take forever to grow?</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18cifbx/how_do_you_deal_with_subborn_nails_that_take/</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>18cg4wg</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Colour changing Sunset Sky nail art I did with thermo gel polish ✨☁️🌆 Swipe for french tips change 😍</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cg4wg</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>18cfv8w</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Sisters nubbins</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cfv8w</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>18cmplv</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Snowflakes</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jxl47bawos4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>18clnjo</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Pink Christmas this year 🩷</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bor2qqvzes4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>18cli80</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>It’s beginning to look a lot like Christmas…</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cli80</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>18clbns</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Holiday Korean Nail Art</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18clbns</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>18ckjyw</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>The best watercolor nails of all time</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y0ssuopy4s4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>18ck5hn</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Christmas spirit 🎄 Nails</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nx3jv1ce1s4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>18cjjh8</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Normally don’t wear red but…</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2mk9z6bvvr4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>18cjaat</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Just wanted to show off my Christmas nails I had done today! I love them!</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cjaat</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>18cix3i</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>My husband bought me new nail stuff and I finally did my nails 🥹</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cix3i</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>18cil30</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Nail glue that will only last a day?</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18cil30/nail_glue_that_will_only_last_a_day/</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>18ci3n4</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>I wanted “Grinchy and green”. Esthetics by Katie in Nova Scotia has done it again!</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ci3n4</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>18ch7ej</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Am I tripping!?! This is a bad overlay right !?!</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ch7ej</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>18ch5n5</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Lacy thermo nails</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/for9q4ykbr4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>18ch4r8</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Any ideas on what to do about this?</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6k9tx8wbbr4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>18cgyng</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Gel paint on my natural nails for the first time ever by myself.</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cgyng</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>18cgxlk</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Are the Amazon polygel brushes as good as Evie's?</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18cgxlk/are_the_amazon_polygel_brushes_as_good_as_evies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>18cgjzz</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>It's officially Christmas time</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cgjzz</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>18cghc1</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Is polygel safer than gel?</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18cghc1/is_polygel_safer_than_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>18cg7gl</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Is there a quick at home fix for messing up the topcoat on a dip manicure?</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18cg7gl/is_there_a_quick_at_home_fix_for_messing_up_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>18cfwag</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happy Holidays </t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yut88kfj1r4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>18cfct2</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Christmas nails! Wine red with gold sparkles for the main set but which of the others should I use for an accent nail?</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yb4xkwkfxq4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>18cf83c</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>My hideous natural nails</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cf83c</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>18ceie9</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>What color should I to do my nails to match this ?</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iq3bjfjyqq4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>18cd8iq</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>My nail tech is fantastic. What I got vs the inspo by amys.clients on Instagram</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cd8iq</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>18caxlc</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>what do i do? ):</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/swl1z9lnzp4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>18cextt</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>got my nails done</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yagvd5h6uq4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>18cerhc</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Getting into the festive mood</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xc52ch0wsq4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>18ce8e9</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Winter nails</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ce8e9</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>18cdyf7</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Make it Christmas but not too Christmas</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ykthm4smq4c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>18cdxgu</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Do you know any good glue for nails?</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18cdxgu/do_you_know_any_good_glue_for_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>18cdn4i</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Simple but sparkly for various holiday parties coming up</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9fufmi7dkq4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>18cdd8c</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Did my own gel nails. Any tips on cleaning up cuticle? My polish lifts after a few days and I’m thinking it’s the cuticles</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yptakrjaiq4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>18cd5yv</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Chipping nails</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d0vdgcwpgq4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>18cd0of</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Possibly unpopular opinion: Kiara Sky Gelly liquids are not my fave.</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18cd0of/possibly_unpopular_opinion_kiara_sky_gelly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>18ccxnd</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Christmas adjacent nails</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ccxnd</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>18cciip</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>I know purple isn't stereotypical Christmas season... but I liked it. The white is sparkles. Happy holidays! ❤️</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cciip</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>18ccezg</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Best Gel Tips for Serious C Curve?</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18ccezg/best_gel_tips_for_serious_c_curve/</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>18ccab7</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>How did I do on my friends nails?</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r22shez1aq4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>18cc14j</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>should i actually push my cuticles up regularly?</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/prot65a18q4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>18cbxi5</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>This weeks nails</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cbxi5</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>18cbtli</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o7q3ox0d6q4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>18cbkck</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>My first set of DIY</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cbkck</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>18cbg0e</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>I posted because I loved these semi cured gels,… but I’m realizing I need a better moisturizer!</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mrnl3f0g3q4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>18cbf1x</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Lost bet, new nails</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/glj3kpi33q4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>18cas7y</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>First time doing my own and I’m so excited to keep improving !!</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cas7y</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>18canjz</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Said goodbye to months of length for musical reasons so here’s my short gel mani for the holidays :’)</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iwg8u9kixp4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>18ca0sk</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Fishnet Stockings ^_^</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fhcdy5ynsp4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>18c8ple</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>cat eye winter wonderland nails ✨💙❄️</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18c8ple</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>18c8p0p</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Girly Christmas nails</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ibcpduloip4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>18c8kra</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Update: i put a thin layer of a holo taco nil polish on top and i already like it much better. It also suits my skin tone better now</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i03phhdshp4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>18c8bjq</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>uv protection</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18c8bjq/uv_protection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>18c6paa</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18c6paa</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>18c6nk1</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Why are my nails getting like this?</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1jy2bu7n2p4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>18c6gja</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>How do I stop this?</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18c6gja</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>18c6m4n</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Christmas set</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v66dqnja2p4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>18c6ih5</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>My Melody Nails</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18c6ih5</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>18c6d47</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Best simple manicure I’ve had in so long</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z552pr380p4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>18c5omw</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Glitter/sequins on hard gel manicure disappearing?</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18c5omw</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>18c3ykn</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Any DIY-er break a nail in the middle of the night and wake up early to fix it before work?</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18c3ykn</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>18c63jx</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Hello Spring! (It’s 32 degrees)</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18c63jx</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>18c63er</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Different design than what I'm always doing, what do you think? I loved it 💛😍</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fc2fwks1yo4c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>18bnw79</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Nail polish won't stay on</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18bnw79/nail_polish_wont_stay_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>18bk1zm</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Is there any reason to buy the “gel art” little bottles?</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xkrigveo2j4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>18c5fe5</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>New winter nails❄️</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8bt499fiso4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>18c4s82</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Sugar Nails🥹🩶🤍</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ku2en4vsmo4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>18c4qd9</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Fire and ice 🧡💙</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18c4qd9</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>18c47q4</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>My first BIAB manicure, is a good result?</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18c47q4</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>18c43w3</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>An uncle on a mission. Did I mention I don't like painting toes?</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kqz0rfdigo4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>18c3zzi</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Do you like watermelons?</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18c3zzi</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>18c3gjw</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>New to gel polishes, here's my first few attempts</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18c3gjw</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>18c3cl5</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Golden Nails ✨️</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/huw0dtu49o4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>18c2ekd</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>First post here - trying new nail polish 💅</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2tooaucxyn4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>18c271m</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>new clawzzzz (€45)</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0bgf3f1jwn4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>18c1z4l</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Pretty colors</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18c1z4l</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>18c0fdj</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>I’m super happy with this design! And just wanted to share.</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8f4ymbkz9n4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>18bzxx3</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Merry Christmas 🎅 🎄</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kivx0h8e3n4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>18bzpnh</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Tried chrome foil for the first time</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bzpnh</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>18cpj6l</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What is the sorcery?? </t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tw0xf9qzht4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>18covzq</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Should I just chop them off &amp; go without polish til they grow out?</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/82ycizmuat4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>18coglx</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>My second attempt at aura nails… I used eyeshadow and covered the imperfections with cats!</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2s79z2l96t4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>18co4ji</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>OPI color comparison</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18co4ji/opi_color_comparison/</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>18cnnmx</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Holiday nails ✨</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vut8v2q6ys4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>18cnh90</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>my black friday haul!</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cnh90</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>18clquq</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Blue cross cuticle remover</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18clquq</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>18clq1d</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Frosty ❄️</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18clq1d</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>18cljt8</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Lemming Lacquer Psyche &amp; Eros ✨️</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cljt8</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>18cky2m</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Best base and top coat for Magnet polishes</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18cky2m/best_base_and_top_coat_for_magnet_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>18ckr62</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Help :( proximal nail fold lifting? it hurts :(</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ckr62</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>18ckn52</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>ILNP Sugarplum Velvet</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1hkmrzjk5s4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>18cjxaf</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>I almost got rid of my magnetic polishes…</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4lr38vm9zr4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>18cjrup</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>💙🩵🤍💝Bath &amp; Body Works💝🤍🩵💙</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cjrup</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>18cjlle</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Trying out my Black Friday polishes! Starting with a deep red for the festive season</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cjlle</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>18cioem</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Zoya - Ivanka and Roxy</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cioem</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>18ciacg</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Help! Need dupes for PPU polishes</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18ciacg/help_need_dupes_for_ppu_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>18chnep</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Green Cat Eyes 💚😻 love a magnetic </t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/a28t3jwddr4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>18chgxm</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Zoya order is in!</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wmpkqvu2er4c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>18cggds</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Is polygel safer than gel?</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18cggds/is_polygel_safer_than_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>18cg8l5</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>wanted a palette cleanser after a summer/fall of long nails [Manucurist Green Flash in Pale Rose]</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ni6ol794r4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>18cg2oz</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Mistletoe &amp; Merlot (focus on the color, not the mess I made of it :)</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3mpufyiy2r4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>18cg09j</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>🎄 Forrest Drive Micro French</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jn0z4xaf2r4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>18cfzli</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>A nice wintery thermal ❄️</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cfzli</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>18cfy5k</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>A holiday miracle!</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2hhnw6oy1r4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>18ce60a</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>ILNP Evermore’s dual personality</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wcubwm98oq4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>18ce2jv</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Loving the colour shift in this polish</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ce2jv</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>18cdt11</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>OMG! I think I found my new favorite polish!</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cdt11</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>18cdhan</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Happy my nails were recorded in my sister's wedding photos</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cdhan</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>18cdex9</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Just a nice neutral!</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cdex9</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>18cd73o</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Because I have little to no self control at times...</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ih092axgq4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>18cd12i</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Trying to get into the holiday spirit ❄️</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mokn269pfq4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>18cbxl9</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>SYS - Weekly Challenge #4 - Sparkling Neutral</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cbxl9</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>18cbu4l</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>my favorite deep red!</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yncfiy9j6q4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>18cbsx9</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Tried the nail blush effect I saw here and loved it!</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cbsx9</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>18cbsnj</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>{PR} I Can’t De-Cider and The Perfect Match by KB Shimmer 😍</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ezhhhde86q4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>18cbigi</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Mooncat Winds of Fate ft. my gremlin wallpaper</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xyqbl7004q4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>18cb3ov</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>A Christmas pomegranate</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cb3ov</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>18capj6</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>They’re not the same, they’re similar!</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yexdoe8yxp4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>18cafr9</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>OPI: Clear your cash</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cafr9</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>18cae7q</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>ether dragon</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cae7q</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>18ca2q3</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Coral Organza</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ca2q3</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>18c9ql0</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Took three hours but it was worth it</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pbltigamqp4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>18c9f85</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>My Blue Velvet Attempt!</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nncfsnm7op4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>18c9f59</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Another day, another velvet post 💚💙💜</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18c9f59</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>18c97k6</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Skinny faux french holiday mess? Sure!</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18c97k6</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>18c921k</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Searching!</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18c921k/searching/</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>18c903i</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Essie Tailored by Twilight</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gpktgob1lp4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>18c8vtr</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>First Post! Spreading the holiday cheer!</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tv362q33kp4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>18c8kfk</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Loving dark jellies for Winter!</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sw300n7qhp4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>18c82kx</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>ILNP Hallucinate (work edition)</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18c82kx</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>18c7j6e</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Kiss Me 💋</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18c7j6e</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>18c630z</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>I wasn’t going for blue-black ballpoint pen ink, but I think I nailed it anyway 😂</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7kkib7mxxo4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>18bu2pd</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Mademoiselle or Mademoiselle?</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bu2pd</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>18bsn6x</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>HELP!! How do I recover from this?</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18bsn6x</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>18c5htl</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Skittle + prugly😍 🎵These are a few of my favorite things🎵</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7e453tw2to4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>18c4pp2</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Black alternative…</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xmm776a5mo4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>18c44aw</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Cursed Pose, Derpy Reindeer</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3rajq09mgo4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>18c3ruc</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>JLLacquer Jellies BF Haul</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18c3ruc</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>18c3l41</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>(Regular polish) first serious attempt at French manicure</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18c3l41</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>18bzpvj</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>PAINK</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t8ou33f80n4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>18cqar7</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>My first time. How did I do?</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cqar7</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>18cpt9m</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Marble Alternative French</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/svyjrawclt4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>18cpsud</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Holiday Nails 🥰</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lvw6jd08lt4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>18cpnn4</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Simple &amp; Cute Gel Manicure</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gh8awrlhjt4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>18cpl6b</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Christmas Gel Nails</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mjcazx9oit4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>18cn34f</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>First time getting cat eye, I have no idea what took me so long. Love it!</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9xuw6ppbss4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>18cmsgv</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Today I made my first white nails, I think I have made a lot of progress in my work</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0tt6p9zops4c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>18cknwr</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>my hello kitty christmas set ˚ʚ♡ɞ˚</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cknwr</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>18ckb5k</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>I tried a new stylist</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ckb5k</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>18cebva</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>First Christmas set of the season</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ktye4mmlpq4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>18cdvtb</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Feeling festive</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f3ndfet8mq4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>18cbwp7</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>My set this week</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cbwp7</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>18c88gg</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>These remind me of the different holiday doors in the nightmare before christmas 🎃❄️🎄☠️ DIY</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b2xeces5fp4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>18c6lrv</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>I don't have a lot of time to do my nails, but I love anything creepy, so I decided to try a red/clear gradient. I didn't have any sponges so I used a finger to blend, and honestly they're my favourite nails ever.</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zzsr8xs72p4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Dec  8 08:08:30 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_12_10.xlsx
+++ b/data/2023_12_10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C772"/>
+  <dimension ref="A1:C937"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13557,6 +13557,2811 @@
         </is>
       </c>
     </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>18di3m2</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>golden✨️✨️</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oi6prsqq315c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>18dgzn9</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holiday set! </t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/a4miy02zp05c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>18dgjy3</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Another pic of this set cause I felt like this image went hard.</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8aexnbmsk05c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>18dgijn</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>did my friend’s christmas nails 🎄</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dgijn</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>18dgeok</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>🍒 for the holidays</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3fa75et4j05c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>18dg8e5</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Painted my cousin’s nails and added bunny stickers! I think they go so well with a cold winter theme!! 🐰💖what do you guys think?</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jyy096c7h05c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>18dfyb8</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Silly Sweet December Nails</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dfyb8</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>18dfxue</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dfxue</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>18dfv5d</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>kawaii christmas</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lgob9lh6d05c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>18dfnkf</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Loveee this set</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b8twym7wa05c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>18dflx2</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>‘tis the szn</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jec9screa05c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>18dflwi</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Beetles gel nail glue</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18dflwi/beetles_gel_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>18dfjl9</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Cute nails for my friend</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dfjl9</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>18dfh5n</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>This design is not the one you are wearing for Christmas, I still have to attend the Christmas shift</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jbzclo2o605c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>18dey6v</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Who’s that Pokémon?</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dey6v</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>18dewmx</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>3yo son</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z4fh0q2c305c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>18depi6</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>My gingerbread winter nails :)</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uhtytx4d105c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>18dellt</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>My old bff did these</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dellt</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>18deffd</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Help is there anyway to fix this?</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2dut3nuoyz4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>18deeaa</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Holiday/winter nails 💅🏻 ❄️</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18deeaa</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>18de706</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>My nail tech was so afraid for the red and purple together, she said she couldn’t possibly make it look good! Well, I think it looks amazing!</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18de706</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>18dd6f5</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>These were my birthday nails! Gel extensions with gel polish.</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dd6f5</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>18dd1iv</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Tips for achieving this natural-but not look?</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ubyelkpclz4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>18dcrbo</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Loving glamnetic press ons recently. What do you think?</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0b8zcbnriz4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>18dc59h</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>I think my brother is undercharging …</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dc59h</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>18dc0g1</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dc0g1</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>18dbyi6</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Christmas party nails!</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/038p3v9abz4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>18dbdj9</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Holiday nails ⛄️❄️</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dbdj9</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>18db7w9</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Press On Nails for Small Nails</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18db7w9/press_on_nails_for_small_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>18db4a2</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>First Fun Manicure 🍒❤️</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gwtf9q1j3z4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>18db383</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Does anyone know of any AFFORDABLE nail polish (gel) brands with pretty/unique bottles?</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18db383/does_anyone_know_of_any_affordable_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>18db2dy</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Green marble nails</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zwognqq23z4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>18db1ka</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>is this a good color on my skin tone?</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rras7j6v2z4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>18daufw</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>✨✨✨</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18daufw</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>18dafhc</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>$20 Upcharge for Gel</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18dafhc/20_upcharge_for_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>18da90i</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Actual metal nail polish</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18da90i</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>18d9z0t</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Not perfect but proud of my natural nails</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o9ecap57ty4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>18d9x7o</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Feeling pretty</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/463f27rqsy4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>18d9nno</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>first time doing nail art, and second time doing gel x tips</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18d9nno</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>18d9ge6</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>In those jeans 👖</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18d9ge6</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>18d923w</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Asymmetrical French with silver foil on a DIY BIAB fill</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q332qzh9ly4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>18d8a4y</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18d8a4y</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>18d8a14</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Need help with a New Years's gift for my girlfriend.</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18d8a14/need_help_with_a_new_yearss_gift_for_my_girlfriend/</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>18d82z1</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>I did my friends nails. Full set polygel. Took 6 hours lol</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18d82z1</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>18d7esg</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>What's a good T H I C C gel top coat?</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18d7esg/whats_a_good_t_h_i_c_c_gel_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>18d6yqh</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>It's beginning to look a lot like Christmas nails 🎄😁</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18d6yqh</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>18d6ukm</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>cute stars on my natural nails at home!</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ese71qd3y4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>18d64ai</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>the first time I use design with cristals</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5tckg70nxx4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>18d5w9t</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Tis the season!</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/345cr5ixvx4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>18d0nqm</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Christmas Nails. I tried 🤷🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n4vn735rqw4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>18d0wpu</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>First Christmas mani of the season 🎄✨</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nhrsxxfqsw4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>18d3ccr</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Advice on flexible nails - Gel doesn't stick!</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18d3ccr/advice_on_flexible_nails_gel_doesnt_stick/</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>18d4rv4</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>My first hard gels ♥️</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rpdop80enx4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>18d4nya</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Can’t decide if I should paint them or leave them nude 🤔</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gp0wksdjmx4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>18d4n4o</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Shape recommendations?</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18d4n4o</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>18d4hlf</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Two months of growth!! (presented by Nail Aid minute acrylics and the kertian one lmao)</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18d4hlf</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>18d43m7</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>How to stop ripping my contacts with long nails</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18d43m7/how_to_stop_ripping_my_contacts_with_long_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>18d3z2s</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Snowy Village ❄️🎄</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gsktrpn6hx4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>18d3yoa</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>First time at home acrylic trial…tips and tricks please 🙏</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18d3yoa</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>18d3p3b</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Mooncat pink skittle to see mean girls musical 💓</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18d3p3b</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>18d3bwq</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Madam Glam - Canada</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18d3bwq/madam_glam_canada/</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>18d3bv9</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Happy holidays! The New Year’s coming 🎉</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/os71wy24cx4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>18d2lzl</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>The best way to model Christmas nails is with a delicious color-matching holiday sugar cookie!! 🍪🎄🎅💅 YUM!</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t37j78xh6x4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>18d273a</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Holiday Nails 🎄❤️❄️</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aei4m6qg3x4c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>18d0zz5</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Wrong shade of nude 🥹😭</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18d0zz5</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>18cyssh</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Starbucks winter set</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cyssh</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>18cx817</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>One red hand, one green. My nail tech is amazing!</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cx817</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>18cuz0p</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>How do you avoid bubbles when putting nail polish?</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18cuz0p/how_do_you_avoid_bubbles_when_putting_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>18crlkh</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Which shape?</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18crlkh</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>18cr7bi</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>My almost Christmas nails</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o3gvgsk23u4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>18d0fpo</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Birthday set!</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/skcx16yxow4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>18cnar6</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Camping Nails</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ocummuqmus4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>18d0bx3</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Were these nails worth the price</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/93y85sc2ow4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>18d092w</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Biab nail journey</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18d092w</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>18d02pn</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Potential 💍 nails</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ugglnq52mw4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>18czsug</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Skittle 💜🤍🖤</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18czsug</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>18czquv</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>This is my first attempt at nail art. I spent way too long on it 🤣</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18czquv</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>18czjgu</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Color is Sea Queen 💅</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wh7iv0bphw4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>18czgyy</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Gifts for 12 yo that loves press on nails?</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18czgyy/gifts_for_12_yo_that_loves_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>18cyc7q</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Winter Sparkle</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6zsdspmx7w4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>18cy5v4</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Did these on myself, how did I do ? I love them, they’re not perfect but I’m getting there!</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cy5v4</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>18cy5o5</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Experimented with my jewelry making supplies. This set is giving me so much life rn!!</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cy5o5</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>18cxyj7</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>First night of Hanukkah nails 💙✨</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cxyj7</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>18cxk26</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>gel polish brands?</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18cxk26/gel_polish_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>18cx5o3</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>What would you pay?</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cx5o3</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>18cx5jv</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>“Do you know the muffin man?”</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cx5jv</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>18cwxg8</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>How did I do?</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6xfoxix6wv4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>18cw0y5</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Christmas nails I did on myself</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mvq1vsr8ov4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>18cvwxv</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>GLOW-in-the-Dark I had awhile back. Still my fav, they were Toxic AF</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cvwxv</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>18cvs6g</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Advice or tips</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18cvs6g/advice_or_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>18cv6kp</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>A dad on a mission. Wow I've been busy lately, but at least they aren't toes.</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cv6kp</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>18cv571</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>My first manicure??... I just like sequins</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ocd6h8ynfv4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>18cuchf</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>My nails are thin and won’t hold polish</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18cuchf/my_nails_are_thin_and_wont_hold_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>18ctxns</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Cute little reindeers!</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1hj0a3gj2v4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>18ct42h</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Simple dark green and gold 🎄🌲</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jsatkk2rsu4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>18crvkh</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>My version of christmas nails. Did them myself 🙈</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fiuizcwgcu4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>18crp3e</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>I'm a little proud of my first try at nail art</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18crp3e</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>18dge7k</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>First time using matte topcoat!</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dge7k</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>18dga5v</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>How to photograph glitter 😩</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dga5v</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>18dfqk0</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>2023 recap</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mgbznq3sb05c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>18dek3w</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Week 1 of Black Friday: ILNP Black Orchid</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dek3w</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>18ddszd</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Dupe recommendations needed!</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18ddszd/dupe_recommendations_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>18ddqia</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Feeling like a sugar plum fairy 🎀🧚‍♀️✨</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ddqia</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>18ddgz0</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Highly obsessed, may get annoying</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wut6o49hpz4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>18dd980</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Sometimes in winter, we wear pink. 💅🏼</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dd980</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>18dd1gd</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Does anyone know how ILNP's Caramel compares to Cirque Colors' Bowery?</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4iijg20clz4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>18dcmh0</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>What's going on with my thumbnail???</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kpxmo8bihz4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>18dciu8</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>🔥Pandemonium🔥</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hhvmuakkgz4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>18dbwqx</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Shout out to the broken nail club</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hj3n2ymtaz4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>18dbwdq</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>The Other Mother 🎂🥧🍭</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dbwdq</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>18dbj0i</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>First time wearing brown polish🤎</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w1gcw36b7z4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>18db8hv</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Frosty blue and spectral lavender</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/20zn52bn4z4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>18dathj</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>✨✨✨</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dathj</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>18dagqy</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>An intense reverse French.</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i6bcs9zmxy4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>18dafkk</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Dark vampy red for Christmas</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jv0a9t6cxy4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>18da3tm</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Actual metal nail polish</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18da3tm</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>18d9nxw</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Where to buy indie nail polish in Southeast Asia?</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18d9nxw/where_to_buy_indie_nail_polish_in_southeast_asia/</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>18d80sd</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Holo Taco - Fruit Punch</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18d80sd</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>18d7x7y</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Why not both??</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18d7x7y</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>18d7vnr</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>thank you for the recommendations!! best drugstore colors?</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18d7vnr/thank_you_for_the_recommendations_best_drugstore/</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>18d7pb1</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Gorgeous but difficult Macchiato Cloud</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18d7pb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>18d6yym</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Beetles gel top coat changing colors?</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18d6yym/beetles_gel_top_coat_changing_colors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>18d6nf1</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Flicker 🔥</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e04qt5vs1y4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>18d5tgw</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>My take on Hanukkah nails</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18d5tgw</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>18d5i5f</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>mooncat antivenom ft my great grandmas loveseat</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hsnc4kwwsx4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>18d5cn4</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>I am such a child when it comes to glow in the dark</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bduux73srx4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>18d52v1</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Looking for suggestions.?</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18d52v1</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>18d4pns</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>A little holiday spirit (just a little)</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18d4pns</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>18d4oc5</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Do you guys cheat?</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18d4oc5</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>18d4hnu</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Loved my nails so much I dyed my hair to match</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dgaa5jy6lx4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>18d4bu7</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Is it just me or is this such a cozy color for winter?</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x0cw4s3wjx4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>18d481p</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Feeling Blue 💙</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18d481p</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>18d3zqh</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>broke my nail while being an anxious mess at the dentist 😩</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ctmj3udbhx4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>18d3x4x</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>ILNP Sugarplum, Cat’s Eye</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0h1lp79rgx4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>18d3wyi</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>So Stinkin’ Cute</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5v8222pngx4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>18d3biv</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Perfect for a rainy winter day</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7cuwpca1cx4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>18d2dam</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Are these looks possible with regular laquer? And what is this style called?</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18d2dam</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>18d27wk</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Let my husband choose my mani</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18d27wk</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>18d18bb</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>There's a pink flash on Zoya "Leia" that makes it a lively sparkly-snow topper.</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18d18bb</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>18d0nlt</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>UV gloves vs. Sunscreen</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18d0nlt/uv_gloves_vs_sunscreen/</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>18d0k9j</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>ILNP “Daydreamer”</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g810w5cypw4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>18cztba</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>first time trying thermal polishes</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cztba</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>18czeu4</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Skittle inspired by sensationails4u 💜🤍🖤</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18czeu4</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>18cynef</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Stickers &amp; Decals Recommendations</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18cynef/stickers_decals_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>18cy0ez</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Looking for dupes for the new MoonCat Collections</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pnkusvl95w4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>18cxt5w</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>(PR) First night of Hanukkah nails 💙✨</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cxt5w</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>18cwkwi</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Finally swatches my whole collection</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m6fv66l7tv4c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>18cvheu</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>There can be only one...</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z5mh9dnwiv4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>18cuy6b</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Im new to the whole thing, but I think they turned out great.</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/irk9y5yhdv4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>18cub9m</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Clearly there's something wrong with my brain... I'm like, they're different!</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cub9m</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>18dggmo</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>First full set of Builder Gel encapsulation!!</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gs8kyebqj05c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>18de2ej</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>i’m trying to get better at stamping, but it’s still a little tricky 😪</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18de2ej</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>18dci1i</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Holiday nails!</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kxfrxs3dgz4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>18dbvp9</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>I might redo the pointer finger</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e3i01pdkaz4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>18db91h</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail art practice! </t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xyb9ifyq4z4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>18da06f</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Manga/anime nails</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18da06f</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>18d8u6u</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Something fun for my clients trip✨🎄</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m94y5k5fjy4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>18d56c9</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>blue &amp; white christmas</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x01lu3wgqx4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>18czlh2</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Second Christmas set from ig fivestarnails.letchworth 🌲</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gh0hqfn6iw4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>18cz88q</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>trying self-nail for the first time</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oqq1nkbyew4c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>18cyuj2</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Starbucks winter set</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cyuj2</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>18cy6oe</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Experimented with my jewelry making supplies. This set is giving me so much life rn!!</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18cy6oe</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>18cuseb</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Glittery pink tartan</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6xwu5vr0cv4c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>18cs6oa</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Latest Christmas set</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jxat8t5lgu4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>18crnmk</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>My first try at nail art</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18crnmk</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Dec  9 08:07:15 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_12_10.xlsx
+++ b/data/2023_12_10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C937"/>
+  <dimension ref="A1:C1092"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16362,6 +16362,2641 @@
         </is>
       </c>
     </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>18e8m0e</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Help finding salon-grade gel polish</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18e8m0e/help_finding_salongrade_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>18e8frd</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Christmas 🎄</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18e8frd</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>18e805y</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>First Russian Manicure</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/78l30kwuy75c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>18e7vkp</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Christmas nails for a Christmas party</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ni8e9tbx75c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>18e7qc9</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Subtly Festive ✨</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6z1cuo1nv75c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>18e6wnj</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>I let my girlfriend pick my nail color (bonus blue light pic)</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18e6wnj</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>18e6pmf</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Simple Xmas Set ❤️💚</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8cpzrs5ej75c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>18e6cm7</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18e6cm7</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>18e64ow</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>matching for the next 3 weeks :)</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ejl0lxzc75c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>18e623q</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Started doing my own gel on natural nails. How can I improve?</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18e623q</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>18e5m8q</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Chrome frenchies for the holidays!</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/chhtfgxj775c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>18e5ivs</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Tis the season</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18e5ivs</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>18e50o6</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Simple Mani for the weekend</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/edveh4e6175c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>18e4rt1</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>my set of press ons for my birthday</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18e4rt1</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>18e4kpl</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Silver stars for the holiday season</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ygxhdlow65c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>18e4bsb</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>What nail shape and length should I get tomorrow?</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18e4bsb</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>18e48la</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>helphelphelphelp</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/92qd3rbat65c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>18e3uc0</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas Festive Nails </t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/26i2ik69p65c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>18e3tre</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/23p0myt8p65c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>18e3oek</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Finally gave myself a fresh set 🥰</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18e3oek</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>18e3bf3</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Wanting to get nails for the first time</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18e3bf3/wanting_to_get_nails_for_the_first_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>18e341o</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>The real reason I put nails on</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18e341o</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>18e2w2g</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Little Debbies are my yearly nail tradition 🎄</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h62w0h76g65c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>18e2oea</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Happy Hanukkah!</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18e2oea</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>18e2ffp</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Little bit seasonal</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nl66x0kub65c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>18e1u96</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>What shape should I do?</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dnnff4ze665c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>18e1rfp</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>My take on Korean style nails! Did I ‘nail‘ it?</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18e1rfp</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>18e10co</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Can you use rubber base gel under BIAB?</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18e10co/can_you_use_rubber_base_gel_under_biab/</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>18dzcq6</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Festive but not toooo holiday!</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/czp8f9hgk55c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>18dz3qf</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Healthiest/long lasting manicures?</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18dz3qf/healthiestlong_lasting_manicures/</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>18dyrm1</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Back with sparkles - bonus: swipe to see the look with flash on!</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dyrm1</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>18dyalr</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Did my friends nails♥️</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dyalr</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>18dy8wn</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>I need to trim my nails, but what shape would look best for them? Does the rounded shape look nice?</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dy8wn</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>18dy8ro</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Merry Chrysler ❤️</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dy8ro</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>18dxv8f</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Forgive my finger nails they’ve been through a lot this week but finger paints “in a glaze” is such a beautiful color! I had to share</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dxv8f</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>18dxrym</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>my fav set i ever had</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y7koralg755c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>18dwzep</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Thought I’d try something different…</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dwzep</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>18dwls8</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>My nails have grown. I need to do maintenance</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ujtdt030y45c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>18dw1at</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>my cranberry nails for christmas 🎄</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h8t47pkdt45c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>18dvx7s</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>🧡🤎 ILNP Caramel and Spiced Cider were made for each other! Perfect for the holiday baking season 🥧</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dvx7s</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>18dvsgb</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Best UK nail growth serums and strengtheners?</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18dvsgb/best_uk_nail_growth_serums_and_strengtheners/</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>18dvmaz</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Decided to start doing one nail in particular.</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vrstzxc2q45c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>18dvkgi</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>DIY birthday nails, how do they look?</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lzuudlynp45c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>18dvj0e</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>A lil geographical survey- gel or acrylic?</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18dvj0e/a_lil_geographical_survey_gel_or_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>18dvccf</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Press On Nail Enthusiasts, How Long Between Sets to Protect Natural Nails?</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18dvccf/press_on_nail_enthusiasts_how_long_between_sets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>18duuf3</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Help me</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18duuf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>18duih8</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>fun christmas nails!</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18duih8</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>18dua0x</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Barbie Chrome</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e6yj8tfbf45c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>18dtxac</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Pretty basic but cute! 🎄💚🤍❤️🤍💚</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dtxac</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>18dtqq0</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What’s your favorite neutral nail color? Mine is DND 867… plus a bit of sparkle ✨ </t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5xik5m8za45c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>18dtoec</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>I'm a machinist so don't do my nails often, but I'm wicked happy with how these turned out!</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t8m4eivfa45c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>18dtano</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Another shot of this perfect shade 💗 So simple, but beautiful.</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u291ronb745c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>18dt4cg</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Cuticles</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dt4cg</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>18dsm7v</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>How much would you pay for these and what can i do better?</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dsm7v</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>18dsc1q</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>My latest set</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dsc1q</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>18ds4d4</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Christmas 🎄❄️ Handpainted</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7grke6cux35c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>18d69yj</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>UV gloves vs. Sunscreen</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18d69yj/uv_gloves_vs_sunscreen/</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>18driey</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Christmas vibes</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oewg65tts35c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>18drggk</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>First acrylic set are they good is bad I paid £40 for them</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18drggk</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>18dm2lj</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>First time doing my nails in over a year</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/biw0qxbkh25c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>18dluw0</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>My ring nail is bending upwards?</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1d0eqiz4f25c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>18dr0c5</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>I started doing my own gel nails back in February - really proud of how far I’ve come!</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eh76rq5ro35c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>18dqtzu</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Opal set</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dqtzu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>18dqq4z</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Green chrome!</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dqq4z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>18d9ud8</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Christmas chrome! Thanks for various inspo sweet friends ❤️</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18d9ud8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>18d9nvs</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Nails got ruined</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xnbhhugfqy4c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>18d7ji2</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Advice for preventing splitting?</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ozokvqss8y4c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>18dpnwg</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Sweater Nails</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bx9l4s0xd35c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>18dp97l</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>My christmas nails❤️</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xi4nwquia35c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>18dp4xj</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Hanukkah gelt 🤎✨</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dp4xj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>18dor2a</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>This month’s, new nail artist finally taking good care of my raging cuticles</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/obvhui28635c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>18dok7o</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Tips on natural nails, more below.</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dok7o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>18doens</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Acrylic nails getting started</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18doens/acrylic_nails_getting_started/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>18dnr9r</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Did my first holiday nails all by myself!</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vn5vghmjx25c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>18dn6su</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>first time trying this effect on my nails</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/27tv9ytgs25c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>18dmlvc</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Barbie nails</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d3mcqhuvm25c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>18dmgaj</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Tips for this kind of broken nail?</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dmgaj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>18dm3sa</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>grinch nail art - handpainted by me!</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xfvxtx3xh25c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>18dlwwm</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Today I was removing my 13th length nails and when we were cutting the nail in half we saw how thick they were OMG!</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ennaevttf25c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>18dlvad</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>first time using gel on myself :)</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dlvad</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>18dl2na</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Had to make short nails for my job but somehow I like it? What do you guys think?</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pskzjzca625c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>18djk41</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Im a beginner nail tech. Critique my first week (pictures in order of when I did them)</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18djk41</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>18djbah</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>My gel X Christmas nails ❄️</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18djbah</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>18dj0xe</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>too long or too cute? ;)</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gxd7g31qr05c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>18dj0kx</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>First christmas set of the year</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0i7jnhmuf15c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>18e7u67</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>lets party! 🌈🖤</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d0ko6pdww75c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>18e7plf</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Subtly Festive</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fivhbgndv75c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>18e64dw</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Tips to keep nails from chipping in the shower?</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18e64dw/tips_to_keep_nails_from_chipping_in_the_shower/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>18e5mph</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>helphelphelphelp</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lmeoh41p775c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>18e39sg</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Dupe for Lights Lacquer Skip It</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18e39sg/dupe_for_lights_lacquer_skip_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>18e2wtz</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Green &amp; gold</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ptmt1mdg65c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>18e2pxd</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Is Fun Lacquer worth the price?</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18e2pxd/is_fun_lacquer_worth_the_price/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>18e2g06</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>I was hospitalized today and after being discharged with good health luckily I decided to treat myself with these three. Not sure if doing a skittle or trying them separately 🤔</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/adqc5j00c65c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>18e1uam</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>They came in!!!</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l9uelj9f665c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>18e1lc8</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Green and Bright 🎶</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18e1lc8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>18e1kk0</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Such a delicate shimmer ✨</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18e1kk0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>18e0zul</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Gotta love that train lighting</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18e0zul</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>18e0vgn</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>if memes aren't allowed then I need to go make r/mani_irl cause this is me</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gtcm2ljlx55c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>18e0l94</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>As 2023 comes to an end: Did you meet, pass, or stay under your nail polish budget?</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18e0l94/as_2023_comes_to_an_end_did_you_meet_pass_or_stay/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>18e0ig3</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Playing with magnets</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18e0ig3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>18e07qf</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>I can't stop starring at it</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18e07qf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>18dzvcv</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Wintery naiks featuring Iggy the Geck</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dzvcv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>18dzswk</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>First set from my Zoya order!</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w3qo6p6co55c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>18dyc04</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Showing Some Grace</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dyc04</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>18dy2bl</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>First ever attempt at a lazy gradient.</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18dy2bl/first_ever_attempt_at_a_lazy_gradient/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>18dy28m</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Looking for good nail polish thinner. What do yall use? 😮</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18dy28m/looking_for_good_nail_polish_thinner_what_do_yall/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>18dxph6</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>I Didn't Say I Would definitively use the winner...</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a3jrn3yu655c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>18dxknb</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Strong iridescent glowy pink topcoat?</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18dxknb/strong_iridescent_glowy_pink_topcoat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>18dwpad</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Festive Velvet Magnetic❤️💚</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j7wsasiqy45c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>18dwnjp</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Feeling very mermaidcore 🧜‍♂️ (Color Club Unicorn Crossing)</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dwnjp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>18dwm8w</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>That blue shift 🤌</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2mukv404y45c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>18dvwhg</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>🧡🤎 ILNP Caramel and Spiced Cider were made for each other! Perfect for the holiday baking season 🥧</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dvwhg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>18dv5d9</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nails were finally hitting their stride and I had to chop them off but I’m still enjoying my first magnetic polish </t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wd1zofddm45c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>18dugvv</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Day 8 of 12 Days of Naild</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/04tcpqsvg45c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>18dudfe</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Holiday looks so far.</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dudfe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>18dtutc</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>ILNP Vaporwave 💅</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dtutc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>18dtr6o</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>ILNP Short Circuit</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dtr6o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>18dtp2l</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>It's no HOH, but very pretty nonetheless</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pkyfnbjka45c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>18dti91</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>tis the season for another mani roundup + honest reviews✨</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dti91</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>18dsul6</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>MVP Nail Saving Tool</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p0w3rocs345c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>18dsret</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Orly Bonder Rubberized base coat, OPI 'Ink', Emily de Molly 'Waiting for the Sun', thick coat of Seche Vite quick dry topcoat.</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w4izwddq245c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>18dsn9c</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Some more shots of Holo Taco’s Party Punch</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dsn9c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>18ds3os</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>3D printed magnet holder for velvet nails</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qnktx79nv35c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>18drmum</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>ILNP - Juliette</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18drmum</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>18dr79n</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Red Chrome nails? Kinda! (China Glaze - Red Pearl)</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dr79n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>18dq0sx</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Why is my nail fold lifting up from the nail?</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g2jzmsprg35c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>18dpxhe</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>a little celebratory glitter for finishing a final ☺️</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9qvoc2f3g35c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>18dpwjf</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Gift for Wife in Pantone Color of the Year 2024</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18dpwjf/gift_for_wife_in_pantone_color_of_the_year_2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>18dpsf3</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>When you can’t decide between red and green - you do both 🎄🎅❄️</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dpsf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>18dpnoz</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>grinch nails handpainted by me! (__kmnails)</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/guzf3tfvd35c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>18dp8ow</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Hanukkah gelt 🤎✨</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dp8ow</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>18dp1q8</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Tortoise Shell Nails</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dp1q8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>18dom8a</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>I had no idea nail polish could look like this</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dom8a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>18doat4</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Jelly Sandwich of a Magnetic Topper!</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nddokxq3235c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>18dn72w</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Underrated gem 🌹</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dn72w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>18dn40u</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>ILNP Bitten + Hex Gradient</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dn40u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>18e727z</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Christmas Gel Nails 🎄</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mzptlwlgn75c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>18e6k1j</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Winter Nails</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18e6k1j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>18e6fdu</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>what would you pay for these?</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18e6fdu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>18e6bxa</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18e6bxa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>18e5uye</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Do you like these bear stickers?? Been using stickers a lot lately to cover up imperfections and complete the look!</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18e5uye</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>18e3uc2</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas Festive Nails </t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8qn9z3u2p65c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>18e3a0m</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>it’s timeee🎄🎄</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j3o2nqluj65c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>18e394m</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Snowy Winter Scene</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9j8r0w6mj65c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>18e2ivf</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>holiday nails</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18e2ivf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>18e2gz6</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Is this chrome?</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rqm2uwv8c65c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>18e1jx3</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Jackson Pollock</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18e1jx3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>18dzlkw</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Christmas without a beautiful red color on your nails would not be a good Christmas</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dzlkw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>18dzh06</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Delicate and beautiful!</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mqp363qhl55c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>18dy3n5</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>my chiikawa princess set! ‹𝟹</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dy3n5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>18du2bz</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Black and white mood</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/700mhcckd45c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>18dr3nm</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>December nails!!</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dr3nm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>18dofeu</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Does anyone else remember Miffy? I’ve been seeing this rabbit everywhere! I did this winter Miffy inspired set on my cousin ❄️ and she was like “No blue” but we love the final result!</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ovadq9h335c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>18djjlr</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Im a beginner nail tech. Critique my first week. (pictures in order of when I did them)</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18djjlr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>18djc4l</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>My Gel X Christmas nails ❄️</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18djc4l</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Dec 10 08:07:34 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_12_10.xlsx
+++ b/data/2023_12_10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1092"/>
+  <dimension ref="A1:C1272"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18997,6 +18997,3066 @@
         </is>
       </c>
     </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>18eyhwu</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Royal Nails Jennie</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xz1we3l3af5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>18eyc3e</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>My Hello Kitty nails</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p2vc1jx08f5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>18ey7eq</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>$150CAD for my X’mas Nails!</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ey7eq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>18exmxm</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Advice - would you be happy with this as an end result?</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18exmxm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>18exfyj</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>What should I name this set as?</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qtmni7e0xe5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>18ex8si</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Candy Cane nails 4 ways! Which one is your fav??</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ex8si</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>18ep5nd</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>1 year since I stopped biting my nails. I’m so proud.</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1cj9n3gelc5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>18eot6x</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Will going to take off my acrylics early damage my nails?</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18eot6x/will_going_to_take_off_my_acrylics_early_damage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>18el18j</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Used another user from here’s pic as my inspo at the salon today</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ae6vxxsbmb5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>18ewq38</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>1 month with IBX nail builder</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ewq38</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>18ewe14</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>My cat's eyes Christmas nails</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ewe14</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>18ewbak</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>DO YOU NEED TO CURE (NON-GEL) NAIL POLISH??? Also, are Shein Nail Press Ons Good?</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18ewbak/do_you_need_to_cure_nongel_nail_polish_also_are/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>18ew6bw</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>something different for me than what I'm used to</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f6fihw0bie5c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>18evrvz</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>First time trying the sponge… Not sure about the result</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18evrvz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>18eva7l</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>spent 250$ after tax and tip for gelx nails. took almost 3 hours and nail tech didnt rush any step. im very satisfied with it but is it overpriced?</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18eva7l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>18ev3l1</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>A little frosty nude</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w71thc2l6e5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>18euhb4</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Did my Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/48izd9nzzd5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>18eua8k</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>They're not perfect but they are finally done</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/828v4lawxd5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>18eu9xz</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Hoping this lasts until Christmas!</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v3i944nsxd5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>18eu9je</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>first time posting, please be gentle. i know my cuticles can be better. natural nails. self manicure. only wearing olive and june nail brightener. i actually love them but still want to improve🤩</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4g27abloxd5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>18et1hi</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Advice on how to tackle this nail crack.</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18et1hi/advice_on_how_to_tackle_this_nail_crack/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>18et1bn</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Is this better?</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3r1v2u94ld5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>18esxz5</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Probably my best set yet</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wn3a4sp7kd5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>18esndt</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>X-mas claws</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z5l509ychd5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>18eslgj</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Yet another set of Christmas nails on your TL! ❄️</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bzd6s3iugd5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>18eshtq</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>First time trying this color, yay or nay?</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/678tdhdufd5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>18esflk</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Gorgeous press ons for this years christmas party🎅🎄❤️✨️</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18esflk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>18eselh</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wish I could capture the true beauty of this topcoat </t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nxhn524yed5c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>18esd6l</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Yay or nay?</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ohtqgsgmed5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>18es862</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Cost for polygel w chrome powder?</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18es862</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>18es782</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Halo Taco | Lite Link + Peely Base | Black Friday Mystery Polish</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k0v33p7xcd5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>18erv49</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>peppermint holiday nails ◡̈</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6wdcl2aq9d5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>18erqsw</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Since the press on sub is no more</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2uf3663m8d5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>18erput</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Looking for this OPI gel color. It is a soft sheer iridescent. TIA</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/07cm95nd8d5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>18er7zd</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Even though I chopped up my cuticles pretty bad I’m so proud of my gel job</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6vrnrk7r3d5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>18er5yl</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>new set!!</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tvymxlv73d5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>18eqv61</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Feelin’ festive 🎄</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18eqv61</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>18eqhjv</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Classic 💅🏻 🥰</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5phsvqj1xc5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>18eplb5</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Winter (but still black) nails!</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18eplb5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>18epkun</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Loving this combo!</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/znerv9u1pc5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>18epbez</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>I did my Christmas nails</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qqkyspnsmc5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>18epb5g</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Not so Christmas nails.</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18epb5g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>18epast</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>I love the cow theme ,I'm in love 😍</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18epast</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>18ep0i8</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Winter Nails</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ajuk5t34kc5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>18eoi5x</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>My first attempt at aurora nails</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5j3wnwlpfc5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>18eod60</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Holiday Nails</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/85jkq2ziec5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>18eoaf1</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>My friend’s nails</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zz3bxegvdc5c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>18enzq0</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>I need help/advice on how to fix my nails after salon</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4xlst63fbc5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>18enovw</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Lovely color, but some say it's fancy😅</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dlon378s8c5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>18enon3</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Had to try velvet nails…</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3e2unlzp8c5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>18enkc7</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>December Set</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/77kzzcno7c5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>18enjkt</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Festive✨</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18enjkt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>18en5us</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Dragon scale nails (made with bubbles) - my nail tech is amazing!</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jygcmaq74c5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>18emzbh</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Snowflakes</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3texe52p2c5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>18emyzt</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Blue chrome rainbows ❄️✨️</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z692onbl2c5c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>18emrq6</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>New Christmas Nails!</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18emrq6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>18emn8j</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Did you really get Christmas nails if you didn’t post them to Reddit?</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tn4se48tzb5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>18em1dr</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Christmas lights 🎄</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jnsq9nooub5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>18em03u</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Did my own nails to try and get into the Christmas spirit.</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ezgzxh3fub5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>18elnqr</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Pink &amp; gold christmas ☃️</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7qp5q8rlrb5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>18elf07</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>This week’s press-ons. Snowflakes!</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fhszx2z2pb5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>18ekmum</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Hanukkah mix &amp; match! 💙✡️✨</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ekmum</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>18ejxw3</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Christmas Nails I did myself</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5xq0ezh6db5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>18ejooe</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Pink Christmas 💖💖</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ejooe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>18ejoe1</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Left handed nail art!</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hji009lzab5c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>18ej9ov</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>I feel like a Christmas ornament lol</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ej9ov</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>18ej83n</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>I need help understanding basics about nails.</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18ej83n/i_need_help_understanding_basics_about_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>18ej7yw</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Just got my nails done</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ej7yw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>18eiyjp</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>I'm going to get my nails done for the first time and I don't know what service to request</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18eiyjp/im_going_to_get_my_nails_done_for_the_first_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>18eix5o</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>What is the best way to do French Tip with regular polish (not gel or dip)? Any tips or product recommendations?</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18eix5o/what_is_the_best_way_to_do_french_tip_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>18eisyk</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Sistaco again</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18eisyk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>18eiman</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>First time using a peach base!</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3of6ys352b5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>18eikwg</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>How much would you charge/pay for these?</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/erw5u55t1b5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>18ei842</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>realizing expectations</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/co7a72ntya5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>18ei4oz</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Tried a new nail place, thoughts?</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ei4oz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>18ei34l</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Polish dupe?</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ei34l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>18ei2dn</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>I asked my nail tech for glitter and Christmas and she delivered!! I would love to see everyone’s Christmas nails!!</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ef8xcjpjxa5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>18ei0s4</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>I need help with crunching nail polish</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ei0s4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>18ehyud</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>I did my own Christmas nails yesterday. First time doing 3D design for the ornament, what do you think?</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ehyud</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>18ehtqs</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Nails</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18ehtqs/nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>18ehsxf</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>My 1st Set Of Christmas Nails 🎄❄️</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ehsxf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>18efvx4</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>What do I ask for when booking?</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18efvx4/what_do_i_ask_for_when_booking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>18ef0ba</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Christmas nails update</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ef0ba</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>18edawh</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>How to function with long natural nails?</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18edawh/how_to_function_with_long_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>18e7b60</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>First Time Doing a French Tip.</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/al9nzpvcq75c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>18dzir0</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Even without an inspo pic, my nail tech always understands the assignment 😍</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t1lz6dsul55c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>18egj29</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18egj29</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>18egfh2</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Nail design tips!?</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18egfh2/nail_design_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>18eg3nd</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18eg3nd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>18duic2</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Nail help</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18duic2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>18dugys</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>Why are my nails chipping?</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18dugys</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>18efuwh</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Christmas green cat eye</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/scfm61dwea5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>18efmdv</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>My grown out nails before and after :) in love</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18efmdv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>18efg6o</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>I wanna see tour holiday nails! Here’s mine</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18efg6o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>18ef5ed</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Christmas nails for my step mum (dark green) and me (white)</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ef5ed</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>18eezj9</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Did my own Christmas Nails!</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18eezj9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>18eez9k</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Ahhh! Loving my Xmas Nails</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5al8jgu07a5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>18eecvf</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>All fixed, again!</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18eecvf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>18eecti</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Chrome for Christmas 23</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18eecti</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>18ee5br</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>My nail tech always indulges my weird ideas</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ee5br</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>18exzgu</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Cirque Morningtide has been on my wishlist for awhile 💙</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4b7ivi9l3f5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>18ewro9</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Ho ho ho</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ewro9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>18ewrld</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Christmasy AF</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bb3o0zq1pe5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>18ewk6u</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>more holiday stuff</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ewk6u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>18ew6af</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>The Perfect Nude?</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ew6af</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>18evuc2</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Repost with Pics</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/G02RLS5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>18evm6t</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Twinkle nail stickers ✨</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18evm6t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>18evf1h</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Snow Day nails</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18evf1h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>18ev8jm</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Badass Berry Scented Polish by I Scream Nails. It does smell like berries!</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hqqaxje28e5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>18etu6e</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>I think this is how I know I have a problem 🙈</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z2b9i0zatd5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>18etq64</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Understated Holiday Vibes</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hzx230s3sd5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>18etce1</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Obsessed with my Zoya polishes</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18etce1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>18et6qk</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Mooncat Artemis Deathkiss: nice formula, meh colour</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18et6qk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>18eszzu</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>UV gel wraps</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18eszzu/uv_gel_wraps/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>18estpk</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>DRK Nails - Donut Give Up</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18estpk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>18esotp</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>💧Mooncat’s Mercury’s Tears💧</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18esotp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>18esjyx</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Love a good cat eye</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18esjyx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>18esgp1</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Country starry night</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18esgp1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>18es6fh</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Halo Taco | Lite Link + Peely Base | Black Friday Mystery Polish</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/euneszqscd5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>18errov</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>ILNP Lolly and Mooncat Artemis’ Deathkiss are shockingly gorgeous together</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8o5hcx9v8d5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>18erlzi</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Got my nails done got my birthday 🥰</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h7uaadlc7d5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>18eqty8</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>My Cirque order came in...</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18eqty8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>18eqcvt</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Starburst jackpot... kinda</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18eqcvt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>18eq91c</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Undecided on if I like this nail shape on me. Thoughts?</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tswcluxwuc5c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>18eq7et</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Gel on top of regular polish? and other combos...</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18eq7et/gel_on_top_of_regular_polish_and_other_combos/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>18epwyg</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>Quick Swatch of "The Seven Ravens" Vapid Lacquer PPU Nov 23</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cngitbwxrc5c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>18epvr9</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Is there anything more satisfying than a swatch ring in rainbow order??</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18epvr9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>18eptmz</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>1961 MAC Factor in Crown Ruby Iridescent</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h3ue1u44rc5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>18ept5l</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Me waiting for my nail polish order that’s out for delivery</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e25beqf0rc5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>18epl82</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Loving this combo!</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mcnbt2x4pc5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>18ep3ra</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>I started doing my own nails because salons always indent my nail beds from pushing too hard during cuticle care. Should I risk it for some beautiful gels while in Korea?</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18ep3ra/i_started_doing_my_own_nails_because_salons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>18ep2oq</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>DVN Moonstone from the Dust to Dust collection🩶simple and understated 🩶</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ep2oq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>18eo85q</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Today I met Walker, the owner of Olive Ave Nails</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18eo85q/today_i_met_walker_the_owner_of_olive_ave_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>18eo6fl</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Fancy Gloss Blueberry Tree Cakes</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18eo6fl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>18ennmp</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>ILNP “Spiced Cider”</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i2m25j5e8c5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>18en3gq</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>My first (and slightly failed 😅) attempt at a skittle, Hanukkah colors! Plus some mini reviews!</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18en3gq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>18emupp</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Full Scream Ahead itch temporarily scratched</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18emupp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>18emg5p</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Electrostatic by Holo Taco pt 2 (with Sonic Unicorn Topper)</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ixh1rjr2yb5c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>18emfak</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Electrostatic by Holo Taco pt 1</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j1417qkvxb5c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>18em9d3</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>They’re not the same, they’re similar! Part two: the swatchening</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18em9d3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>18em3g1</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Love that warm shimmer 🌟</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18em3g1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>18eljn0</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Anyone buy polish from Etsy sellers before?</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18eljn0/anyone_buy_polish_from_etsy_sellers_before/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>18ekztn</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Did you do your own wedding nails?</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ekztn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>18eksyc</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Inverted glitter mani</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18eksyc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>18ekr6z</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Winter Nails? Ice Queen? Sparkly Snowflakes</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ekr6z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>18ekgpd</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Remember those old-school glittery Christmas cards?</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e11dcwphhb5c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>18ekd6a</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Mooncat’s Access Denied</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zqgmf2btgb5c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>18ek6v1</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>Holiday party nails</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ek6v1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>18ek3sh</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Did I get a bad bottle or are my eyes just broken?</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ek3sh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>18ej6bd</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Cirque changed Lavender Sky????</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ej6bd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>18ej293</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>confetti 🎉</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ej293</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>18eim1y</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>In love with this unusual brown + purple effect</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/azyjtzx22b5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>18eiemq</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Today’s mani</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18eiemq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>18eid9d</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>BKL nail mail</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18eid9d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>18eib1a</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Mocha</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18eib1a/mocha/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>18ehqfk</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>My 1st Set Of Christmas Nails 🎄❄️🎄</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ehqfk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>18eheym</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>My nails and roses matched so I had to get pictures 💕</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18eheym</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>18eaai5</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Clap!...or Clash!!</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18eaai5/clapor_clash/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>18egqdw</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Matching in the wild: trail shoe edition</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fc9tblzdma5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>18e1wpg</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Is this chrome?</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gwm1iqk1765c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>18egfbu</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Feelin’ festive 🎄</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18egfbu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>18efjmb</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>☕️ Triple Shot, Please ☕️</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18efjmb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>18efepg</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>2023 lacquer in review.</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18efepg/2023_lacquer_in_review/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>18ef8tf</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>The pictures don’t do it justice</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ef8tf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>18eec97</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>Ready to snatch 🩷</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3p8dnwny0a5c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>18ee1lc</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Simple white mani</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ee1lc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>18ec5d2</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Getting obsessed with chromes again</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://imgur.com/f9idGlP</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>18e9la9</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f14h0fi1j85c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>18e8sp2</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>This stunnig vintage oil slick brown to green shift from the now defunct Sephora polish line I just found while cleaning out a box</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6mjclbkw885c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>18euhag</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>My attempt at winter nails</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vntj4kozzd5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>18etd3d</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Xmas nails done by me🐻‍❄️</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18etd3d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>18eszqs</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>❄️❄️</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nxds7jxokd5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>18esw69</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Lavender cow print frenchies with glitter</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18esw69</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>18erltf</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Illustration-style snowflakes and candy canes</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6cxjtl0b7d5c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>18eov5o</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>First ever nail art</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xu5tu3ouic5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>18ekoec</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Vintage glittery Christmas cards 😍 painted by moi </t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2t77i66cjb5c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>18ejmsh</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Left handed nail art</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1pu3s2tnab5c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>18eh69t</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Christmas! (They're supposed to be antlers)</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18eh69t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>18ecw86</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>This took me 5 hours…</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1dbhk2ihm95c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>18ec0cg</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>Christmassy Tartan Nails 🎄 (by charlylouisebeauty)</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iv0tnpcjc95c1.png</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>